<commit_message>
FIX-#2596: Fix xlsx file
Signed-off-by: Igoshev, Yaroslav <yaroslav.igoshev@intel.com>
</commit_message>
<xml_diff>
--- a/modin/pandas/test/data/excel_sheetname_title.xlsx
+++ b/modin/pandas/test/data/excel_sheetname_title.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/DevinPetersohn/software_builds/modin/modin/pandas/test/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yigoshev\repo\modin\modin\pandas\test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C9B2B0-0260-3A45-B063-8579DF07736A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{020BEDA1-5C11-4D35-9E4F-5F050461AC14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11580" yWindow="5460" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{E3595E16-348B-A246-B7B8-8221A649A08D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{E3595E16-348B-A246-B7B8-8221A649A08D}"/>
   </bookViews>
   <sheets>
     <sheet name="SpecialName" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="SecondSpecialName" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -417,7 +418,7 @@
 </a:theme>
 </file>
 
-<file path=xl/worksheets/Sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{771FC97F-797C-0247-8579-94E984FB5DD1}">
   <dimension ref="A1:H31"/>
   <sheetViews>
@@ -425,9 +426,9 @@
       <selection sqref="A1:H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -453,7 +454,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -479,7 +480,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -505,7 +506,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -531,7 +532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -557,7 +558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -583,7 +584,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -609,7 +610,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -635,7 +636,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -661,7 +662,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -687,7 +688,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>0</v>
       </c>
@@ -713,7 +714,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1</v>
       </c>
@@ -739,7 +740,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2</v>
       </c>
@@ -765,7 +766,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>3</v>
       </c>
@@ -791,7 +792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>4</v>
       </c>
@@ -817,7 +818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>5</v>
       </c>
@@ -843,7 +844,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>6</v>
       </c>
@@ -869,7 +870,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>7</v>
       </c>
@@ -895,7 +896,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>8</v>
       </c>
@@ -921,7 +922,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>9</v>
       </c>
@@ -947,7 +948,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>0</v>
       </c>
@@ -973,7 +974,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>1</v>
       </c>
@@ -999,7 +1000,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2</v>
       </c>
@@ -1025,7 +1026,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>3</v>
       </c>
@@ -1051,7 +1052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>4</v>
       </c>
@@ -1077,7 +1078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>5</v>
       </c>
@@ -1103,7 +1104,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>6</v>
       </c>
@@ -1129,7 +1130,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>7</v>
       </c>
@@ -1155,7 +1156,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>8</v>
       </c>
@@ -1181,7 +1182,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>9</v>
       </c>
@@ -1207,7 +1208,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>0</v>
       </c>
@@ -1235,10 +1236,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/Sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDE4D774-29E9-8D45-80A1-3454CEFA94FD}">
   <dimension ref="A1:H9"/>
   <sheetViews>
@@ -1246,9 +1248,9 @@
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1274,7 +1276,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1300,7 +1302,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1326,7 +1328,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1352,7 +1354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1378,7 +1380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1404,7 +1406,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1430,7 +1432,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1456,7 +1458,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1484,10 +1486,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/Sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AF0CD86-AA23-4A4A-B061-B2C9A62DA63F}">
   <dimension ref="A1:H23"/>
   <sheetViews>
@@ -1495,9 +1498,9 @@
       <selection activeCell="H13" sqref="A13:H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1523,7 +1526,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1549,7 +1552,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1575,7 +1578,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1601,7 +1604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1627,7 +1630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1653,7 +1656,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1679,7 +1682,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1705,7 +1708,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1731,7 +1734,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1741,7 +1744,7 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1751,7 +1754,7 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1761,7 +1764,7 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1771,7 +1774,7 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1781,7 +1784,7 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1791,7 +1794,7 @@
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1801,7 +1804,7 @@
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1811,7 +1814,7 @@
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1821,7 +1824,7 @@
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1831,7 +1834,7 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1843,10 +1846,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/Sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB459E74-F35C-7241-BDD3-95274687B39C}">
   <dimension ref="A1:B31"/>
   <sheetViews>
@@ -1854,9 +1858,9 @@
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1864,7 +1868,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>4</v>
       </c>
@@ -1872,7 +1876,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>5</v>
       </c>
@@ -1880,7 +1884,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>6</v>
       </c>
@@ -1888,7 +1892,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>7</v>
       </c>
@@ -1896,7 +1900,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>8</v>
       </c>
@@ -1904,7 +1908,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>9</v>
       </c>
@@ -1912,7 +1916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>0</v>
       </c>
@@ -1920,7 +1924,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1928,7 +1932,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2</v>
       </c>
@@ -1936,7 +1940,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>3</v>
       </c>
@@ -1944,7 +1948,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>4</v>
       </c>
@@ -1952,7 +1956,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>5</v>
       </c>
@@ -1960,7 +1964,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>6</v>
       </c>
@@ -1968,7 +1972,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>7</v>
       </c>
@@ -1976,7 +1980,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>8</v>
       </c>
@@ -1984,7 +1988,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>9</v>
       </c>
@@ -1992,7 +1996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>0</v>
       </c>
@@ -2000,7 +2004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1</v>
       </c>
@@ -2008,7 +2012,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2</v>
       </c>
@@ -2016,7 +2020,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>3</v>
       </c>
@@ -2024,7 +2028,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>4</v>
       </c>
@@ -2032,7 +2036,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>5</v>
       </c>
@@ -2040,7 +2044,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>6</v>
       </c>
@@ -2048,7 +2052,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>7</v>
       </c>
@@ -2056,7 +2060,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>8</v>
       </c>
@@ -2064,7 +2068,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>9</v>
       </c>
@@ -2072,7 +2076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>0</v>
       </c>
@@ -2080,7 +2084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>1</v>
       </c>
@@ -2088,7 +2092,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>2</v>
       </c>
@@ -2096,7 +2100,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>3</v>
       </c>
@@ -2106,5 +2110,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
FIX-#2596: Revert excel file
Signed-off-by: Igoshev, Yaroslav <yaroslav.igoshev@intel.com>
</commit_message>
<xml_diff>
--- a/modin/pandas/test/data/excel_sheetname_title.xlsx
+++ b/modin/pandas/test/data/excel_sheetname_title.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yigoshev\repo\modin\modin\pandas\test\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/DevinPetersohn/software_builds/modin/modin/pandas/test/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{020BEDA1-5C11-4D35-9E4F-5F050461AC14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C9B2B0-0260-3A45-B063-8579DF07736A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{E3595E16-348B-A246-B7B8-8221A649A08D}"/>
+    <workbookView xWindow="11580" yWindow="5460" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{E3595E16-348B-A246-B7B8-8221A649A08D}"/>
   </bookViews>
   <sheets>
     <sheet name="SpecialName" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <sheet name="SecondSpecialName" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -418,7 +417,7 @@
 </a:theme>
 </file>
 
-<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/Sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{771FC97F-797C-0247-8579-94E984FB5DD1}">
   <dimension ref="A1:H31"/>
   <sheetViews>
@@ -426,9 +425,9 @@
       <selection sqref="A1:H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -454,7 +453,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -480,7 +479,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -506,7 +505,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -532,7 +531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -558,7 +557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -584,7 +583,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -610,7 +609,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -636,7 +635,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -662,7 +661,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -688,7 +687,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>0</v>
       </c>
@@ -714,7 +713,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1</v>
       </c>
@@ -740,7 +739,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
@@ -766,7 +765,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>3</v>
       </c>
@@ -792,7 +791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>4</v>
       </c>
@@ -818,7 +817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>5</v>
       </c>
@@ -844,7 +843,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>6</v>
       </c>
@@ -870,7 +869,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>7</v>
       </c>
@@ -896,7 +895,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>8</v>
       </c>
@@ -922,7 +921,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>9</v>
       </c>
@@ -948,7 +947,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>0</v>
       </c>
@@ -974,7 +973,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1000,7 +999,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2</v>
       </c>
@@ -1026,7 +1025,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>3</v>
       </c>
@@ -1052,7 +1051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>4</v>
       </c>
@@ -1078,7 +1077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>5</v>
       </c>
@@ -1104,7 +1103,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>6</v>
       </c>
@@ -1130,7 +1129,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>7</v>
       </c>
@@ -1156,7 +1155,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>8</v>
       </c>
@@ -1182,7 +1181,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>9</v>
       </c>
@@ -1208,7 +1207,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>0</v>
       </c>
@@ -1236,11 +1235,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/Sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDE4D774-29E9-8D45-80A1-3454CEFA94FD}">
   <dimension ref="A1:H9"/>
   <sheetViews>
@@ -1248,9 +1246,9 @@
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1276,7 +1274,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1302,7 +1300,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1328,7 +1326,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1354,7 +1352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1380,7 +1378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1406,7 +1404,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1432,7 +1430,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1458,7 +1456,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1486,11 +1484,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/Sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AF0CD86-AA23-4A4A-B061-B2C9A62DA63F}">
   <dimension ref="A1:H23"/>
   <sheetViews>
@@ -1498,9 +1495,9 @@
       <selection activeCell="H13" sqref="A13:H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1526,7 +1523,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1552,7 +1549,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1578,7 +1575,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1604,7 +1601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1630,7 +1627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1656,7 +1653,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1682,7 +1679,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1708,7 +1705,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1734,7 +1731,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1744,7 +1741,7 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1754,7 +1751,7 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1764,7 +1761,7 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1774,7 +1771,7 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1784,7 +1781,7 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1794,7 +1791,7 @@
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1804,7 +1801,7 @@
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1814,7 +1811,7 @@
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1824,7 +1821,7 @@
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1834,7 +1831,7 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1846,11 +1843,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/Sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB459E74-F35C-7241-BDD3-95274687B39C}">
   <dimension ref="A1:B31"/>
   <sheetViews>
@@ -1858,9 +1854,9 @@
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1868,7 +1864,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>4</v>
       </c>
@@ -1876,7 +1872,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>5</v>
       </c>
@@ -1884,7 +1880,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>6</v>
       </c>
@@ -1892,7 +1888,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>7</v>
       </c>
@@ -1900,7 +1896,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>8</v>
       </c>
@@ -1908,7 +1904,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>9</v>
       </c>
@@ -1916,7 +1912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>0</v>
       </c>
@@ -1924,7 +1920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1932,7 +1928,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2</v>
       </c>
@@ -1940,7 +1936,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>3</v>
       </c>
@@ -1948,7 +1944,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>4</v>
       </c>
@@ -1956,7 +1952,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>5</v>
       </c>
@@ -1964,7 +1960,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>6</v>
       </c>
@@ -1972,7 +1968,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>7</v>
       </c>
@@ -1980,7 +1976,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>8</v>
       </c>
@@ -1988,7 +1984,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>9</v>
       </c>
@@ -1996,7 +1992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>0</v>
       </c>
@@ -2004,7 +2000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1</v>
       </c>
@@ -2012,7 +2008,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2</v>
       </c>
@@ -2020,7 +2016,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>3</v>
       </c>
@@ -2028,7 +2024,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>4</v>
       </c>
@@ -2036,7 +2032,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>5</v>
       </c>
@@ -2044,7 +2040,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>6</v>
       </c>
@@ -2052,7 +2048,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>7</v>
       </c>
@@ -2060,7 +2056,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>8</v>
       </c>
@@ -2068,7 +2064,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>9</v>
       </c>
@@ -2076,7 +2072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>0</v>
       </c>
@@ -2084,7 +2080,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1</v>
       </c>
@@ -2092,7 +2088,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>2</v>
       </c>
@@ -2100,7 +2096,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>3</v>
       </c>
@@ -2110,6 +2106,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>